<commit_message>
docs: incl. dummy entries for args in .xlsx
</commit_message>
<xml_diff>
--- a/overview/potential_output.xlsx
+++ b/overview/potential_output.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Data_Science/CorrelAid/Data_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Data_Science/CorrelAid/datenguide-python/overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE0F121-9F4F-1C4F-A782-3075BBCCC82F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCF07D2-14A9-FD4B-9798-7CE6D133695E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{FF57D526-EE65-C245-BFAB-848701ABE567}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>tc={FE343922-9A81-E74A-B75B-8992E59EAE62}</author>
   </authors>
   <commentList>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{220E84EB-8B41-5749-BAFC-230F22D19CA7}">
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{220E84EB-8B41-5749-BAFC-230F22D19CA7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -47,7 +47,7 @@
     default?</t>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{FE343922-9A81-E74A-B75B-8992E59EAE62}">
+    <comment ref="N6" authorId="1" shapeId="0" xr:uid="{FE343922-9A81-E74A-B75B-8992E59EAE62}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
   <si>
     <t>Code</t>
   </si>
@@ -120,13 +120,25 @@
   </si>
   <si>
     <t>Dummy outline for a potential output of the data overview.</t>
+  </si>
+  <si>
+    <t>arg1</t>
+  </si>
+  <si>
+    <t>arg2</t>
+  </si>
+  <si>
+    <t>1 or True</t>
+  </si>
+  <si>
+    <t>0 or False</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,12 +192,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,7 +240,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1"/>
@@ -243,6 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -566,10 +573,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L6" dT="2020-03-16T15:13:12.23" personId="{47FEADE8-FEBC-DC4A-8EA0-FC5C285F0BEF}" id="{220E84EB-8B41-5749-BAFC-230F22D19CA7}">
+  <threadedComment ref="M6" dT="2020-03-16T15:13:12.23" personId="{47FEADE8-FEBC-DC4A-8EA0-FC5C285F0BEF}" id="{220E84EB-8B41-5749-BAFC-230F22D19CA7}">
     <text>default?</text>
   </threadedComment>
-  <threadedComment ref="M6" dT="2020-03-16T15:13:19.24" personId="{47FEADE8-FEBC-DC4A-8EA0-FC5C285F0BEF}" id="{FE343922-9A81-E74A-B75B-8992E59EAE62}">
+  <threadedComment ref="N6" dT="2020-03-16T15:13:19.24" personId="{47FEADE8-FEBC-DC4A-8EA0-FC5C285F0BEF}" id="{FE343922-9A81-E74A-B75B-8992E59EAE62}">
     <text>??</text>
   </threadedComment>
 </ThreadedComments>
@@ -577,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0DC9EE-9D82-9A43-AF45-BB856396FF9E}">
-  <dimension ref="B1:O35"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -590,7 +597,7 @@
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="21" thickBot="1">
+    <row r="1" spans="2:16" ht="21" thickBot="1">
       <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
@@ -602,16 +609,16 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="2:15" ht="17" thickTop="1"/>
-    <row r="3" spans="2:15">
+    <row r="2" spans="2:16" ht="17" thickTop="1"/>
+    <row r="3" spans="2:16">
       <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:16">
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="2:15" ht="18" thickBot="1">
+    <row r="5" spans="2:16" ht="18" thickBot="1">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -636,16 +643,21 @@
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="L5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="2:15" ht="17" thickTop="1">
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:16" ht="17" thickTop="1">
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
@@ -665,15 +677,21 @@
         <f>I6-H6</f>
         <v>17</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="K6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="2:15">
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="2:16">
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
@@ -689,14 +707,20 @@
       <c r="I7">
         <v>2017</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="K7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:16">
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
@@ -706,8 +730,14 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="K8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
@@ -717,8 +747,14 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:15">
+      <c r="K9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
@@ -728,8 +764,14 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="K10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
@@ -739,8 +781,14 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="K11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
@@ -750,8 +798,14 @@
       <c r="E12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="K12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
@@ -761,8 +815,14 @@
       <c r="E13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="K13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
@@ -772,8 +832,14 @@
       <c r="E14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:15">
+      <c r="K14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="C15" s="6" t="s">
         <v>13</v>
       </c>
@@ -783,8 +849,14 @@
       <c r="E15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="K15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
@@ -794,8 +866,14 @@
       <c r="E16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="3:5">
+      <c r="K16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
       <c r="C17" s="6" t="s">
         <v>13</v>
       </c>
@@ -805,8 +883,14 @@
       <c r="E17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="3:5">
+      <c r="K17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12">
       <c r="C18" s="6" t="s">
         <v>13</v>
       </c>
@@ -816,8 +900,14 @@
       <c r="E18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="3:5">
+      <c r="K18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12">
       <c r="C19" s="6" t="s">
         <v>13</v>
       </c>
@@ -827,8 +917,14 @@
       <c r="E19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="3:5">
+      <c r="K19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12">
       <c r="C20" s="6" t="s">
         <v>13</v>
       </c>
@@ -839,7 +935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
+    <row r="21" spans="3:12">
       <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
@@ -850,7 +946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="3:12">
       <c r="C22" s="6" t="s">
         <v>14</v>
       </c>
@@ -861,7 +957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="3:12">
       <c r="C23" s="6" t="s">
         <v>14</v>
       </c>
@@ -872,7 +968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="3:12">
       <c r="C24" s="6" t="s">
         <v>14</v>
       </c>
@@ -883,7 +979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="3:5">
+    <row r="25" spans="3:12">
       <c r="C25" s="6" t="s">
         <v>14</v>
       </c>
@@ -894,7 +990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
+    <row r="26" spans="3:12">
       <c r="C26" s="6" t="s">
         <v>14</v>
       </c>
@@ -905,7 +1001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
+    <row r="27" spans="3:12">
       <c r="C27" s="6" t="s">
         <v>14</v>
       </c>
@@ -916,7 +1012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="3:12">
       <c r="C28" s="6" t="s">
         <v>14</v>
       </c>
@@ -927,7 +1023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" spans="3:12">
       <c r="C29" s="6" t="s">
         <v>14</v>
       </c>
@@ -938,7 +1034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
+    <row r="30" spans="3:12">
       <c r="C30" s="6" t="s">
         <v>14</v>
       </c>
@@ -949,7 +1045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
+    <row r="31" spans="3:12">
       <c r="C31" s="6" t="s">
         <v>14</v>
       </c>
@@ -960,7 +1056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="3:5">
+    <row r="32" spans="3:12">
       <c r="C32" s="6" t="s">
         <v>14</v>
       </c>

</xml_diff>